<commit_message>
update robot auth&crud test
</commit_message>
<xml_diff>
--- a/auth.test/users.xlsx
+++ b/auth.test/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttser\OneDrive\เดสก์ท็อป\RPA_Robot Framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttser\OneDrive\เดสก์ท็อป\RPA_Robot Framework\auth.test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A115047-4445-4D27-B911-E3152117A846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB412B26-E126-4E79-841F-79E8AAAA62D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -38,19 +38,13 @@
   </si>
   <si>
     <t>user3</t>
-  </si>
-  <si>
-    <t>user4</t>
-  </si>
-  <si>
-    <t>$2b$10$abcdefghijklmnopqrstuv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +56,12 @@
       <b/>
       <sz val="11"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,18 +454,11 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>